<commit_message>
Added presentation and the other documentation for the project
</commit_message>
<xml_diff>
--- a/Machine learning/DigitsRecognizer/output.xlsx
+++ b/Machine learning/DigitsRecognizer/output.xlsx
@@ -518,7 +518,7 @@
         <v>0.981326530612245</v>
       </c>
       <c r="I3">
-        <v>3533.789527893066</v>
+        <v>2749.29559135437</v>
       </c>
       <c r="J3">
         <v>0.9819047619047619</v>
@@ -550,7 +550,7 @@
         <v>0.9672789115646256</v>
       </c>
       <c r="I4">
-        <v>18.94172048568726</v>
+        <v>17.84076809883118</v>
       </c>
       <c r="J4">
         <v>0.9705555555555555</v>

</xml_diff>